<commit_message>
Started creating the functionality for the append information.
</commit_message>
<xml_diff>
--- a/ExcelReader/data/Example.xlsx
+++ b/ExcelReader/data/Example.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="85">
   <si>
     <t>t</t>
   </si>
@@ -261,6 +261,18 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>Log File</t>
+  </si>
+  <si>
+    <t>log_entries.txt</t>
+  </si>
+  <si>
+    <t>Gen*FuelCons</t>
+  </si>
+  <si>
+    <t>GenConfig[3-6]</t>
   </si>
 </sst>
 </file>
@@ -616,10 +628,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,7 +682,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1814400</v>
+        <v>360000</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -732,6 +744,23 @@
       </c>
       <c r="D10" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -740,7 +769,7 @@
       <formula1>",,,,,Community Name,input,output"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A11">
-      <formula1>",,,,,Community Name,input,output"</formula1>
+      <formula1>",,,,,Community Name,Template,input,output"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -754,7 +783,7 @@
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,7 +1067,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Updated the add in to include the Log File information.
</commit_message>
<xml_diff>
--- a/ExcelReader/data/Example.xlsx
+++ b/ExcelReader/data/Example.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="84">
   <si>
     <t>t</t>
   </si>
@@ -254,15 +254,9 @@
     <t>Gen8IdealPctP</t>
   </si>
   <si>
-    <t>template</t>
-  </si>
-  <si>
     <t>C:\SVN_Simon\radical_pwcsolar\Development\trunk\ExcelReader\data\testTemplate.xls</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>Log File</t>
   </si>
   <si>
@@ -273,6 +267,9 @@
   </si>
   <si>
     <t>GenConfig[3-6]</t>
+  </si>
+  <si>
+    <t>Template</t>
   </si>
 </sst>
 </file>
@@ -631,7 +628,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,7 +679,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>360000</v>
+        <v>1209600</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -734,42 +731,45 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" t="s">
         <v>78</v>
-      </c>
-      <c r="B10" t="s">
-        <v>79</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
         <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A12">
-      <formula1>",,,,,Community Name,input,output"</formula1>
-    </dataValidation>
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A11">
       <formula1>",,,,,Community Name,Template,input,output"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B9">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A12">
+      <formula1>",,,,,Community Name,Template,,input,output"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A10">
+      <formula1>",,,,,Community Name,,,input,output,Template"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added percent complete progress chart to SimResults and status bar; tidied simulator percent complete output.
</commit_message>
<xml_diff>
--- a/ExcelReader/data/Example.xlsx
+++ b/ExcelReader/data/Example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="210" windowWidth="20730" windowHeight="8130"/>
+    <workbookView xWindow="120" yWindow="270" windowWidth="20730" windowHeight="8070" tabRatio="725" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="4" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="StationStats" sheetId="2" r:id="rId3"/>
     <sheet name="GenConfigurations" sheetId="3" r:id="rId4"/>
     <sheet name="Solar" sheetId="5" r:id="rId5"/>
+    <sheet name="SimResults" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="86">
   <si>
     <t>t</t>
   </si>
@@ -47,9 +48,6 @@
     <t>daly river 1s.csv</t>
   </si>
   <si>
-    <t>weekly.csv</t>
-  </si>
-  <si>
     <t>week</t>
   </si>
   <si>
@@ -92,9 +90,6 @@
     <t>output</t>
   </si>
   <si>
-    <t>GenOverload</t>
-  </si>
-  <si>
     <t>Gen1MaxP</t>
   </si>
   <si>
@@ -185,9 +180,6 @@
     <t>GenConfig19</t>
   </si>
   <si>
-    <t>Gen*Cnt</t>
-  </si>
-  <si>
     <t>Gen1MinRunTPa</t>
   </si>
   <si>
@@ -215,12 +207,6 @@
     <t>daly river Pv 1s.csv</t>
   </si>
   <si>
-    <t>StatBlackCnt</t>
-  </si>
-  <si>
-    <t>PvECnt</t>
-  </si>
-  <si>
     <t>PvSetMaxDownP</t>
   </si>
   <si>
@@ -254,9 +240,6 @@
     <t>Gen8IdealPctP</t>
   </si>
   <si>
-    <t>C:\SVN_Simon\radical_pwcsolar\Development\trunk\ExcelReader\data\testTemplate.xls</t>
-  </si>
-  <si>
     <t>Log File</t>
   </si>
   <si>
@@ -270,6 +253,30 @@
   </si>
   <si>
     <t>Template</t>
+  </si>
+  <si>
+    <t>Init...</t>
+  </si>
+  <si>
+    <t>This sheet is automatically filled.  Any edits will be lost each time you run the Simulator</t>
+  </si>
+  <si>
+    <t>Analyser.xlsx</t>
+  </si>
+  <si>
+    <t>Gen*RunCnt</t>
+  </si>
+  <si>
+    <t>analyse.csv</t>
+  </si>
+  <si>
+    <t>Percent Complete</t>
+  </si>
+  <si>
+    <t>Run 3000000 iterations...</t>
+  </si>
+  <si>
+    <t>inner loop took 14.6575341s</t>
   </si>
 </sst>
 </file>
@@ -314,7 +321,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -322,6 +329,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -335,6 +343,155 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-AU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SimResults!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Percent Complete</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>SimResults!$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="33223424"/>
+        <c:axId val="33224960"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="33223424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="33224960"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="33224960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="33223424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -625,16 +782,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
@@ -644,45 +801,45 @@
     <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1209600</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -690,38 +847,29 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
       <c r="D8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -729,32 +877,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E11" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -765,11 +913,11 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B9">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A12">
-      <formula1>",,,,,Community Name,Template,,input,output"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A10">
       <formula1>",,,,,Community Name,,,input,output,Template"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A12">
+      <formula1>",,,,,Community Name,,,input,output"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -803,109 +951,109 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I1" t="s">
+      <c r="T1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>21</v>
-      </c>
-      <c r="R1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="U1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="X1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="Z1" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA1" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB1" s="6" t="s">
-        <v>63</v>
-      </c>
       <c r="AC1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH1" t="s">
         <v>70</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AI1" t="s">
         <v>71</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AJ1" t="s">
         <v>72</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
@@ -1040,10 +1188,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1082,61 +1230,61 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
         <v>36</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>37</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>38</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>39</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>40</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>41</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>42</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>43</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>44</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>45</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>46</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>47</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>48</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>49</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>50</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>51</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>52</v>
-      </c>
-      <c r="S1" t="s">
-        <v>53</v>
-      </c>
-      <c r="T1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -1234,10 +1382,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1254,4 +1402,47 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated Analyst and Simulator as shown to PWC today.
</commit_message>
<xml_diff>
--- a/ExcelReader/data/Example.xlsx
+++ b/ExcelReader/data/Example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="270" windowWidth="20730" windowHeight="8070" tabRatio="725" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="330" windowWidth="20730" windowHeight="8010" tabRatio="725"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="87">
   <si>
     <t>t</t>
   </si>
@@ -249,34 +249,37 @@
     <t>Gen*FuelCons</t>
   </si>
   <si>
-    <t>GenConfig[3-6]</t>
-  </si>
-  <si>
     <t>Template</t>
   </si>
   <si>
+    <t>Analyser.xlsx</t>
+  </si>
+  <si>
+    <t>analyse.csv</t>
+  </si>
+  <si>
+    <t>Run 3000000 iterations...</t>
+  </si>
+  <si>
+    <t>*Cnt</t>
+  </si>
+  <si>
+    <t>This sheet is automatically filled.  Any edits will be lost each time you run the Simulator</t>
+  </si>
+  <si>
     <t>Init...</t>
   </si>
   <si>
-    <t>This sheet is automatically filled.  Any edits will be lost each time you run the Simulator</t>
-  </si>
-  <si>
-    <t>Analyser.xlsx</t>
-  </si>
-  <si>
-    <t>Gen*RunCnt</t>
-  </si>
-  <si>
-    <t>analyse.csv</t>
-  </si>
-  <si>
     <t>Percent Complete</t>
   </si>
   <si>
-    <t>Run 3000000 iterations...</t>
-  </si>
-  <si>
-    <t>inner loop took 14.6575341s</t>
+    <t>Run started on 22/10/2012 4:40:39 PM</t>
+  </si>
+  <si>
+    <t>inner loop took 15.771577s</t>
+  </si>
+  <si>
+    <t>GenConfig*</t>
   </si>
 </sst>
 </file>
@@ -375,7 +378,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>SimResults!$A$4</c:f>
+              <c:f>SimResults!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -387,7 +390,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>SimResults!$B$4</c:f>
+              <c:f>SimResults!$B$5</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -408,11 +411,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="33223424"/>
-        <c:axId val="33224960"/>
+        <c:axId val="153325952"/>
+        <c:axId val="153327488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="33223424"/>
+        <c:axId val="153325952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -421,7 +424,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="33224960"/>
+        <c:crossAx val="153327488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -429,7 +432,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="33224960"/>
+        <c:axId val="153327488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -442,7 +445,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="33223424"/>
+        <c:crossAx val="153325952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -476,7 +479,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="7" name="Chart 6"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -784,15 +787,13 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.5703125" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -860,13 +861,13 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -879,13 +880,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" t="s">
         <v>77</v>
       </c>
-      <c r="B10" t="s">
-        <v>80</v>
-      </c>
       <c r="C10" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -902,11 +903,11 @@
         <v>75</v>
       </c>
       <c r="E11" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A11">
       <formula1>",,,,,Community Name,Template,input,output"</formula1>
     </dataValidation>
@@ -915,9 +916,6 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A10">
       <formula1>",,,,,Community Name,,,input,output,Template"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A12">
-      <formula1>",,,,,Community Name,,,input,output"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1407,37 +1405,44 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B4" s="7">
-        <v>1</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- deleted old xlsm file - update Example & macros with Start Date - PWCSLMS-11 Enhance accepted input time formats - PWCSLMS-12 Value scaling over time - included sample Analyser.xls - included some simple tests
</commit_message>
<xml_diff>
--- a/ExcelReader/data/Example.xlsx
+++ b/ExcelReader/data/Example.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="89">
   <si>
     <t>t</t>
   </si>
@@ -280,12 +280,21 @@
   </si>
   <si>
     <t>GenConfig*</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Start Time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -324,7 +333,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -333,6 +342,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -363,7 +374,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -411,11 +421,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="153325952"/>
-        <c:axId val="153327488"/>
+        <c:axId val="149926272"/>
+        <c:axId val="149927808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153325952"/>
+        <c:axId val="149926272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -424,7 +434,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153327488"/>
+        <c:crossAx val="149927808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -432,7 +442,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153327488"/>
+        <c:axId val="149927808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -445,7 +455,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153325952"/>
+        <c:crossAx val="149926272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -785,14 +795,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="4" width="13.5703125" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
@@ -803,15 +815,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
+      <c r="B1" s="8"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -834,88 +847,114 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>3000000</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="B5" s="9">
+        <v>40909</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B6" s="8">
+        <v>3000000</v>
+      </c>
+      <c r="C6" s="8"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="b">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>73</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>74</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>23</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>75</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>86</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+    </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A11">
-      <formula1>",,,,,Community Name,Template,input,output"</formula1>
+      <formula1>",,,,,Community Name,,,input,output,Template"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B10">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A10">
-      <formula1>",,,,,Community Name,,,input,output,Template"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A6">
+      <formula1>",,,iterations,,,,,input,output,,Community Name"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A13">
+      <formula1>",,,,,Community Name,,,input,output,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A12">
+      <formula1>",,,,,,,,input,output,Start Time,Log File"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A5">
+      <formula1>",,,,,,,,input,output,Start Time,Community Name"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fuel efficiency curves, updated manual.
</commit_message>
<xml_diff>
--- a/ExcelReader/data/Example.xlsx
+++ b/ExcelReader/data/Example.xlsx
@@ -4,22 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="330" windowWidth="20730" windowHeight="8010" tabRatio="725"/>
+    <workbookView xWindow="120" yWindow="330" windowWidth="20730" windowHeight="8010" tabRatio="725" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="4" r:id="rId1"/>
     <sheet name="GenStats" sheetId="1" r:id="rId2"/>
-    <sheet name="StationStats" sheetId="2" r:id="rId3"/>
-    <sheet name="GenConfigurations" sheetId="3" r:id="rId4"/>
-    <sheet name="Solar" sheetId="5" r:id="rId5"/>
-    <sheet name="SimResults" sheetId="6" r:id="rId6"/>
+    <sheet name="FuelEfficiency" sheetId="7" r:id="rId3"/>
+    <sheet name="StationStats" sheetId="2" r:id="rId4"/>
+    <sheet name="GenConfigurations" sheetId="3" r:id="rId5"/>
+    <sheet name="Solar" sheetId="5" r:id="rId6"/>
+    <sheet name="SimResults" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="161">
   <si>
     <t>t</t>
   </si>
@@ -63,30 +64,6 @@
     <t>GenAvailCfg</t>
   </si>
   <si>
-    <t>Gen1FuelCons</t>
-  </si>
-  <si>
-    <t>Gen2FuelCons</t>
-  </si>
-  <si>
-    <t>Gen3FuelCons</t>
-  </si>
-  <si>
-    <t>Gen4FuelCons</t>
-  </si>
-  <si>
-    <t>Gen5FuelCons</t>
-  </si>
-  <si>
-    <t>Gen6FuelCons</t>
-  </si>
-  <si>
-    <t>Gen7FuelCons</t>
-  </si>
-  <si>
-    <t>Gen8FuelCons</t>
-  </si>
-  <si>
     <t>output</t>
   </si>
   <si>
@@ -258,34 +235,274 @@
     <t>analyse.csv</t>
   </si>
   <si>
+    <t>*Cnt</t>
+  </si>
+  <si>
+    <t>This sheet is automatically filled.  Any edits will be lost each time you run the Simulator</t>
+  </si>
+  <si>
+    <t>GenConfig*</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Start Time</t>
+  </si>
+  <si>
+    <t>Gen1FuelCons1P</t>
+  </si>
+  <si>
+    <t>Gen1FuelCons1L</t>
+  </si>
+  <si>
+    <t>Gen1FuelCons2P</t>
+  </si>
+  <si>
+    <t>Gen1FuelCons2L</t>
+  </si>
+  <si>
+    <t>Gen1FuelCons3P</t>
+  </si>
+  <si>
+    <t>Gen1FuelCons3L</t>
+  </si>
+  <si>
+    <t>Gen1FuelCons4P</t>
+  </si>
+  <si>
+    <t>Gen1FuelCons4L</t>
+  </si>
+  <si>
+    <t>Gen1FuelCons5P</t>
+  </si>
+  <si>
+    <t>Gen1FuelCons5L</t>
+  </si>
+  <si>
+    <t>Gen2FuelCons1P</t>
+  </si>
+  <si>
+    <t>Gen2FuelCons1L</t>
+  </si>
+  <si>
+    <t>Gen2FuelCons2P</t>
+  </si>
+  <si>
+    <t>Gen2FuelCons2L</t>
+  </si>
+  <si>
+    <t>Gen2FuelCons3P</t>
+  </si>
+  <si>
+    <t>Gen2FuelCons3L</t>
+  </si>
+  <si>
+    <t>Gen2FuelCons4P</t>
+  </si>
+  <si>
+    <t>Gen2FuelCons4L</t>
+  </si>
+  <si>
+    <t>Gen2FuelCons5P</t>
+  </si>
+  <si>
+    <t>Gen2FuelCons5L</t>
+  </si>
+  <si>
+    <t>Gen3FuelCons1P</t>
+  </si>
+  <si>
+    <t>Gen3FuelCons1L</t>
+  </si>
+  <si>
+    <t>Gen3FuelCons2P</t>
+  </si>
+  <si>
+    <t>Gen3FuelCons2L</t>
+  </si>
+  <si>
+    <t>Gen3FuelCons3P</t>
+  </si>
+  <si>
+    <t>Gen3FuelCons3L</t>
+  </si>
+  <si>
+    <t>Gen3FuelCons4P</t>
+  </si>
+  <si>
+    <t>Gen3FuelCons4L</t>
+  </si>
+  <si>
+    <t>Gen3FuelCons5P</t>
+  </si>
+  <si>
+    <t>Gen3FuelCons5L</t>
+  </si>
+  <si>
+    <t>Gen4FuelCons1P</t>
+  </si>
+  <si>
+    <t>Gen4FuelCons1L</t>
+  </si>
+  <si>
+    <t>Gen4FuelCons2P</t>
+  </si>
+  <si>
+    <t>Gen4FuelCons2L</t>
+  </si>
+  <si>
+    <t>Gen4FuelCons3P</t>
+  </si>
+  <si>
+    <t>Gen4FuelCons3L</t>
+  </si>
+  <si>
+    <t>Gen4FuelCons4P</t>
+  </si>
+  <si>
+    <t>Gen4FuelCons4L</t>
+  </si>
+  <si>
+    <t>Gen4FuelCons5P</t>
+  </si>
+  <si>
+    <t>Gen4FuelCons5L</t>
+  </si>
+  <si>
+    <t>Gen5FuelCons1P</t>
+  </si>
+  <si>
+    <t>Gen5FuelCons1L</t>
+  </si>
+  <si>
+    <t>Gen5FuelCons2P</t>
+  </si>
+  <si>
+    <t>Gen5FuelCons2L</t>
+  </si>
+  <si>
+    <t>Gen5FuelCons3P</t>
+  </si>
+  <si>
+    <t>Gen5FuelCons3L</t>
+  </si>
+  <si>
+    <t>Gen5FuelCons4P</t>
+  </si>
+  <si>
+    <t>Gen5FuelCons4L</t>
+  </si>
+  <si>
+    <t>Gen5FuelCons5P</t>
+  </si>
+  <si>
+    <t>Gen5FuelCons5L</t>
+  </si>
+  <si>
+    <t>Gen6FuelCons1P</t>
+  </si>
+  <si>
+    <t>Gen6FuelCons1L</t>
+  </si>
+  <si>
+    <t>Gen6FuelCons2P</t>
+  </si>
+  <si>
+    <t>Gen6FuelCons2L</t>
+  </si>
+  <si>
+    <t>Gen6FuelCons3P</t>
+  </si>
+  <si>
+    <t>Gen6FuelCons3L</t>
+  </si>
+  <si>
+    <t>Gen6FuelCons4P</t>
+  </si>
+  <si>
+    <t>Gen6FuelCons4L</t>
+  </si>
+  <si>
+    <t>Gen6FuelCons5P</t>
+  </si>
+  <si>
+    <t>Gen6FuelCons5L</t>
+  </si>
+  <si>
+    <t>Gen7FuelCons1P</t>
+  </si>
+  <si>
+    <t>Gen7FuelCons1L</t>
+  </si>
+  <si>
+    <t>Gen7FuelCons2P</t>
+  </si>
+  <si>
+    <t>Gen7FuelCons2L</t>
+  </si>
+  <si>
+    <t>Gen7FuelCons3P</t>
+  </si>
+  <si>
+    <t>Gen7FuelCons3L</t>
+  </si>
+  <si>
+    <t>Gen7FuelCons4P</t>
+  </si>
+  <si>
+    <t>Gen7FuelCons4L</t>
+  </si>
+  <si>
+    <t>Gen7FuelCons5P</t>
+  </si>
+  <si>
+    <t>Gen7FuelCons5L</t>
+  </si>
+  <si>
+    <t>Gen8FuelCons1P</t>
+  </si>
+  <si>
+    <t>Gen8FuelCons1L</t>
+  </si>
+  <si>
+    <t>Gen8FuelCons2P</t>
+  </si>
+  <si>
+    <t>Gen8FuelCons2L</t>
+  </si>
+  <si>
+    <t>Gen8FuelCons3P</t>
+  </si>
+  <si>
+    <t>Gen8FuelCons3L</t>
+  </si>
+  <si>
+    <t>Gen8FuelCons4P</t>
+  </si>
+  <si>
+    <t>Gen8FuelCons4L</t>
+  </si>
+  <si>
+    <t>Gen8FuelCons5P</t>
+  </si>
+  <si>
+    <t>Gen8FuelCons5L</t>
+  </si>
+  <si>
+    <t>Init...</t>
+  </si>
+  <si>
     <t>Run 3000000 iterations...</t>
   </si>
   <si>
-    <t>*Cnt</t>
-  </si>
-  <si>
-    <t>This sheet is automatically filled.  Any edits will be lost each time you run the Simulator</t>
-  </si>
-  <si>
-    <t>Init...</t>
-  </si>
-  <si>
     <t>Percent Complete</t>
   </si>
   <si>
-    <t>Run started on 22/10/2012 4:40:39 PM</t>
-  </si>
-  <si>
-    <t>inner loop took 15.771577s</t>
-  </si>
-  <si>
-    <t>GenConfig*</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Start Time</t>
+    <t>Run started on 7/11/2012 5:15:34 PM</t>
+  </si>
+  <si>
+    <t>inner loop took 17.1447143s</t>
   </si>
 </sst>
 </file>
@@ -341,9 +558,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -374,6 +591,167 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Gen 1 Fuel Efficiency (L/kWh</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-AU" baseline="0"/>
+              <a:t> vs LF)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:marker>
+              <c:symbol val="diamond"/>
+              <c:size val="7"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(FuelEfficiency!$B$2,FuelEfficiency!$D$2,FuelEfficiency!$F$2,FuelEfficiency!$H$2,FuelEfficiency!$J$2)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(FuelEfficiency!$C$2,FuelEfficiency!$E$2,FuelEfficiency!$G$2,FuelEfficiency!$I$2,FuelEfficiency!$K$2)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="71249280"/>
+        <c:axId val="71349376"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="71249280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="71349376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="71349376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="71249280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-AU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -421,11 +799,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="149926272"/>
-        <c:axId val="149927808"/>
+        <c:axId val="71324800"/>
+        <c:axId val="71336320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="149926272"/>
+        <c:axId val="71324800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -434,7 +812,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149927808"/>
+        <c:crossAx val="71336320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -442,7 +820,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="149927808"/>
+        <c:axId val="71336320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -455,7 +833,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149926272"/>
+        <c:crossAx val="71324800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -476,6 +854,41 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>42861</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>485774</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>2</xdr:row>
@@ -489,7 +902,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -795,10 +1208,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,16 +1228,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="7"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -847,22 +1260,22 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B5" s="9">
+        <v>75</v>
+      </c>
+      <c r="B5" s="8">
         <v>40909</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7">
         <v>3000000</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -871,90 +1284,96 @@
       <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>78</v>
+        <v>14</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
-        <v>87</v>
+      <c r="B10" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" t="s">
         <v>73</v>
       </c>
-      <c r="B12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" t="s">
-        <v>75</v>
-      </c>
-      <c r="E12" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="7"/>
     </row>
   </sheetData>
-  <dataValidations count="6">
+  <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A11">
       <formula1>",,,,,Community Name,,,input,output,Template"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B10">
-      <formula1>"Yes, No"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A6">
       <formula1>",,,iterations,,,,,input,output,,Community Name"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A13">
-      <formula1>",,,,,Community Name,,,input,output,"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A12">
       <formula1>",,,,,,,,input,output,Start Time,Log File"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A5">
       <formula1>",,,,,,,,input,output,Start Time,Community Name"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A13">
+      <formula1>",,,,,Community Name,,,input,output,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B10">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A15">
+      <formula1>",,,,,Community Name,,,input,output,"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -965,7 +1384,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AJ2"/>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
@@ -976,124 +1395,99 @@
     <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
     <col min="2" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="28" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="36" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="20" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="28" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="I1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R1" t="s">
-        <v>21</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="W1" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="X1" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y1" s="6" t="s">
+      <c r="K1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="U1" t="s">
         <v>57</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="V1" t="s">
         <v>58</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="W1" t="s">
         <v>59</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="X1" t="s">
         <v>60</v>
       </c>
-      <c r="AC1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="Y1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1125,81 +1519,57 @@
         <v>255</v>
       </c>
       <c r="K2">
-        <v>0.3</v>
+        <v>240</v>
       </c>
       <c r="L2">
-        <v>0.3</v>
+        <v>3600</v>
       </c>
       <c r="M2">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>3600</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="V2">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="X2">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="Y2">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="Z2">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="AA2">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="AB2">
-        <v>0</v>
-      </c>
-      <c r="AC2">
-        <v>40</v>
-      </c>
-      <c r="AD2">
-        <v>40</v>
-      </c>
-      <c r="AE2">
-        <v>40</v>
-      </c>
-      <c r="AF2">
-        <v>40</v>
-      </c>
-      <c r="AG2">
-        <v>40</v>
-      </c>
-      <c r="AH2">
-        <v>40</v>
-      </c>
-      <c r="AI2">
-        <v>40</v>
-      </c>
-      <c r="AJ2">
         <v>40</v>
       </c>
     </row>
@@ -1209,6 +1579,515 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet7"/>
+  <dimension ref="A1:CC2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="14" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" t="s">
+        <v>86</v>
+      </c>
+      <c r="M1" t="s">
+        <v>87</v>
+      </c>
+      <c r="N1" t="s">
+        <v>88</v>
+      </c>
+      <c r="O1" t="s">
+        <v>89</v>
+      </c>
+      <c r="P1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>91</v>
+      </c>
+      <c r="R1" t="s">
+        <v>92</v>
+      </c>
+      <c r="S1" t="s">
+        <v>93</v>
+      </c>
+      <c r="T1" t="s">
+        <v>94</v>
+      </c>
+      <c r="U1" t="s">
+        <v>95</v>
+      </c>
+      <c r="V1" t="s">
+        <v>96</v>
+      </c>
+      <c r="W1" t="s">
+        <v>97</v>
+      </c>
+      <c r="X1" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>126</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>127</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>128</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>129</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>130</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>131</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>132</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>133</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>134</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>135</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>136</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>137</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>138</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>139</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>140</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>141</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>142</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>143</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>144</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>145</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>146</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>147</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>148</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>149</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>150</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>151</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>152</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>153</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>154</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0.4</v>
+      </c>
+      <c r="D2">
+        <v>0.1</v>
+      </c>
+      <c r="E2">
+        <v>0.3</v>
+      </c>
+      <c r="F2">
+        <v>0.3</v>
+      </c>
+      <c r="G2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H2">
+        <v>0.8</v>
+      </c>
+      <c r="I2">
+        <v>0.31</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>0.35</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0.4</v>
+      </c>
+      <c r="N2">
+        <v>0.1</v>
+      </c>
+      <c r="O2">
+        <v>0.3</v>
+      </c>
+      <c r="P2">
+        <v>0.3</v>
+      </c>
+      <c r="Q2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="R2">
+        <v>0.8</v>
+      </c>
+      <c r="S2">
+        <v>0.31</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>0.35</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0.4</v>
+      </c>
+      <c r="X2">
+        <v>0.1</v>
+      </c>
+      <c r="Y2">
+        <v>0.3</v>
+      </c>
+      <c r="Z2">
+        <v>0.3</v>
+      </c>
+      <c r="AA2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AB2">
+        <v>0.8</v>
+      </c>
+      <c r="AC2">
+        <v>0.31</v>
+      </c>
+      <c r="AD2">
+        <v>1</v>
+      </c>
+      <c r="AE2">
+        <v>0.35</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0.4</v>
+      </c>
+      <c r="AH2">
+        <v>0.1</v>
+      </c>
+      <c r="AI2">
+        <v>0.3</v>
+      </c>
+      <c r="AJ2">
+        <v>0.3</v>
+      </c>
+      <c r="AK2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AL2">
+        <v>0.8</v>
+      </c>
+      <c r="AM2">
+        <v>0.31</v>
+      </c>
+      <c r="AN2">
+        <v>1</v>
+      </c>
+      <c r="AO2">
+        <v>0.35</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <v>0.4</v>
+      </c>
+      <c r="AR2">
+        <v>0.1</v>
+      </c>
+      <c r="AS2">
+        <v>0.3</v>
+      </c>
+      <c r="AT2">
+        <v>0.3</v>
+      </c>
+      <c r="AU2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AV2">
+        <v>0.8</v>
+      </c>
+      <c r="AW2">
+        <v>0.31</v>
+      </c>
+      <c r="AX2">
+        <v>1</v>
+      </c>
+      <c r="AY2">
+        <v>0.35</v>
+      </c>
+      <c r="AZ2">
+        <v>0</v>
+      </c>
+      <c r="BA2">
+        <v>0.4</v>
+      </c>
+      <c r="BB2">
+        <v>0.1</v>
+      </c>
+      <c r="BC2">
+        <v>0.3</v>
+      </c>
+      <c r="BD2">
+        <v>0.3</v>
+      </c>
+      <c r="BE2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="BF2">
+        <v>0.8</v>
+      </c>
+      <c r="BG2">
+        <v>0.31</v>
+      </c>
+      <c r="BH2">
+        <v>1</v>
+      </c>
+      <c r="BI2">
+        <v>0.35</v>
+      </c>
+      <c r="BJ2">
+        <v>0</v>
+      </c>
+      <c r="BK2">
+        <v>0.4</v>
+      </c>
+      <c r="BL2">
+        <v>0.1</v>
+      </c>
+      <c r="BM2">
+        <v>0.3</v>
+      </c>
+      <c r="BN2">
+        <v>0.3</v>
+      </c>
+      <c r="BO2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="BP2">
+        <v>0.8</v>
+      </c>
+      <c r="BQ2">
+        <v>0.31</v>
+      </c>
+      <c r="BR2">
+        <v>1</v>
+      </c>
+      <c r="BS2">
+        <v>0.35</v>
+      </c>
+      <c r="BT2">
+        <v>0</v>
+      </c>
+      <c r="BU2">
+        <v>0.4</v>
+      </c>
+      <c r="BV2">
+        <v>0.1</v>
+      </c>
+      <c r="BW2">
+        <v>0.3</v>
+      </c>
+      <c r="BX2">
+        <v>0.3</v>
+      </c>
+      <c r="BY2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="BZ2">
+        <v>0.8</v>
+      </c>
+      <c r="CA2">
+        <v>0.31</v>
+      </c>
+      <c r="CB2">
+        <v>1</v>
+      </c>
+      <c r="CC2">
+        <v>0.35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C2"/>
@@ -1225,10 +2104,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1247,7 +2126,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:T2"/>
@@ -1267,61 +2146,61 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
+      <c r="K1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="L1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
+      <c r="M1" t="s">
         <v>37</v>
       </c>
-      <c r="F1" t="s">
+      <c r="N1" t="s">
         <v>38</v>
       </c>
-      <c r="G1" t="s">
+      <c r="O1" t="s">
         <v>39</v>
       </c>
-      <c r="H1" t="s">
+      <c r="P1" t="s">
         <v>40</v>
       </c>
-      <c r="I1" t="s">
+      <c r="Q1" t="s">
         <v>41</v>
       </c>
-      <c r="J1" t="s">
+      <c r="R1" t="s">
         <v>42</v>
       </c>
-      <c r="K1" t="s">
+      <c r="S1" t="s">
         <v>43</v>
       </c>
-      <c r="L1" t="s">
+      <c r="T1" t="s">
         <v>44</v>
-      </c>
-      <c r="M1" t="s">
-        <v>45</v>
-      </c>
-      <c r="N1" t="s">
-        <v>46</v>
-      </c>
-      <c r="O1" t="s">
-        <v>47</v>
-      </c>
-      <c r="P1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>49</v>
-      </c>
-      <c r="R1" t="s">
-        <v>50</v>
-      </c>
-      <c r="S1" t="s">
-        <v>51</v>
-      </c>
-      <c r="T1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -1395,7 +2274,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:C2"/>
@@ -1419,10 +2298,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1441,48 +2320,48 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B5" s="7">
+        <v>158</v>
+      </c>
+      <c r="B5" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- more unit tests for the simulator - updated manual - updated analyser
</commit_message>
<xml_diff>
--- a/ExcelReader/data/Example.xlsx
+++ b/ExcelReader/data/Example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="330" windowWidth="20730" windowHeight="8010" tabRatio="725" activeTab="6"/>
+    <workbookView xWindow="120" yWindow="330" windowWidth="16005" windowHeight="7605" tabRatio="725"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="4" r:id="rId1"/>
@@ -610,6 +610,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -687,11 +688,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="71249280"/>
-        <c:axId val="71349376"/>
+        <c:axId val="148216832"/>
+        <c:axId val="147841792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71249280"/>
+        <c:axId val="148216832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -703,12 +704,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71349376"/>
+        <c:crossAx val="147841792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71349376"/>
+        <c:axId val="147841792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -719,7 +720,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71249280"/>
+        <c:crossAx val="148216832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -799,11 +800,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="71324800"/>
-        <c:axId val="71336320"/>
+        <c:axId val="147904768"/>
+        <c:axId val="147910656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="71324800"/>
+        <c:axId val="147904768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -812,7 +813,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71336320"/>
+        <c:crossAx val="147910656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -820,7 +821,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71336320"/>
+        <c:axId val="147910656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -833,7 +834,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71324800"/>
+        <c:crossAx val="147904768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1210,9 +1211,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1353,7 +1352,7 @@
       <c r="B14" s="7"/>
     </row>
   </sheetData>
-  <dataValidations count="7">
+  <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A11">
       <formula1>",,,,,Community Name,,,input,output,Template"</formula1>
     </dataValidation>
@@ -1366,13 +1365,19 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A5">
       <formula1>",,,,,,,,input,output,Start Time,Community Name"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A13">
-      <formula1>",,,,,Community Name,,,input,output,"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B10">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A15">
+      <formula1>",,,,,Community Name,,,input,output,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A16">
+      <formula1>",,,,,Community Name,,,input,output,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A13">
+      <formula1>",,,,,Community Name,,,input,output,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A14">
       <formula1>",,,,,Community Name,,,input,output,"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1583,7 +1588,9 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:CC2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2325,9 +2332,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
- fixed renaming of template output csv file which stopped the template being generated - fixed axis scaling for Excel 2003 & 2010 - stopped auto-updating charts and formulas in template helper sheet - fixed bug where stale excel was left running after specific COM error message - new xls and xlsx files
</commit_message>
<xml_diff>
--- a/ExcelReader/data/Example.xlsx
+++ b/ExcelReader/data/Example.xlsx
@@ -499,10 +499,10 @@
     <t>Percent Complete</t>
   </si>
   <si>
-    <t>Run started on 7/11/2012 5:15:34 PM</t>
-  </si>
-  <si>
-    <t>inner loop took 17.1447143s</t>
+    <t>Run started on 23/11/2012 11:07:28 AM</t>
+  </si>
+  <si>
+    <t>inner loop took 16.9206919s</t>
   </si>
 </sst>
 </file>
@@ -688,11 +688,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="148216832"/>
-        <c:axId val="147841792"/>
+        <c:axId val="48513792"/>
+        <c:axId val="48515712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="148216832"/>
+        <c:axId val="48513792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -704,12 +704,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147841792"/>
+        <c:crossAx val="48515712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="147841792"/>
+        <c:axId val="48515712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -720,7 +720,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148216832"/>
+        <c:crossAx val="48513792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -800,11 +800,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="147904768"/>
-        <c:axId val="147910656"/>
+        <c:axId val="106110336"/>
+        <c:axId val="106140800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="147904768"/>
+        <c:axId val="106110336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -813,7 +813,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147910656"/>
+        <c:crossAx val="106140800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -821,7 +821,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147910656"/>
+        <c:axId val="106140800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -834,7 +834,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147904768"/>
+        <c:crossAx val="106110336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -903,7 +903,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1391,9 +1391,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1588,9 +1586,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:CC2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2138,9 +2134,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2286,9 +2280,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
rename *ECnt to *E
</commit_message>
<xml_diff>
--- a/ExcelReader/data/Example.xlsx
+++ b/ExcelReader/data/Example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="330" windowWidth="16005" windowHeight="7605" tabRatio="725"/>
+    <workbookView xWindow="120" yWindow="330" windowWidth="16005" windowHeight="7605" tabRatio="725" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="4" r:id="rId1"/>
@@ -688,11 +688,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="48513792"/>
-        <c:axId val="48515712"/>
+        <c:axId val="145439744"/>
+        <c:axId val="149172992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48513792"/>
+        <c:axId val="145439744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -704,12 +704,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48515712"/>
+        <c:crossAx val="149172992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48515712"/>
+        <c:axId val="149172992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -720,7 +720,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48513792"/>
+        <c:crossAx val="145439744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -800,11 +800,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="106110336"/>
-        <c:axId val="106140800"/>
+        <c:axId val="88070784"/>
+        <c:axId val="88076672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="106110336"/>
+        <c:axId val="88070784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -813,7 +813,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106140800"/>
+        <c:crossAx val="88076672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -821,7 +821,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106140800"/>
+        <c:axId val="88076672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -834,7 +834,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106110336"/>
+        <c:crossAx val="88070784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1211,7 +1211,9 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2095,7 +2097,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
fixed fuel usage and other minor touchups.
</commit_message>
<xml_diff>
--- a/ExcelReader/data/Example.xlsx
+++ b/ExcelReader/data/Example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="330" windowWidth="16005" windowHeight="7605" tabRatio="725" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="390" windowWidth="16005" windowHeight="7545" tabRatio="725"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="168">
   <si>
     <t>t</t>
   </si>
@@ -223,9 +223,6 @@
     <t>log_entries.txt</t>
   </si>
   <si>
-    <t>Gen*FuelCons</t>
-  </si>
-  <si>
     <t>Template</t>
   </si>
   <si>
@@ -493,16 +490,40 @@
     <t>Init...</t>
   </si>
   <si>
-    <t>Run 3000000 iterations...</t>
-  </si>
-  <si>
     <t>Percent Complete</t>
   </si>
   <si>
-    <t>Run started on 23/11/2012 11:07:28 AM</t>
-  </si>
-  <si>
-    <t>inner loop took 16.9206919s</t>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>output.csv</t>
+  </si>
+  <si>
+    <t>Run 100000 iterations...</t>
+  </si>
+  <si>
+    <t>Run started on 10/01/2013 5:21:08 PM</t>
+  </si>
+  <si>
+    <t>Solar Load Model  Copyright (C) 2012, 2013  Power Water Corporation.</t>
+  </si>
+  <si>
+    <t>This program comes with ABSOLUTELY NO WARRANTY;</t>
+  </si>
+  <si>
+    <t>This is free software, and you are welcome to redistribute it</t>
+  </si>
+  <si>
+    <t>under certain conditions; see the file COPYING for details.</t>
+  </si>
+  <si>
+    <t>inner loop took 11.6191618s</t>
+  </si>
+  <si>
+    <t>*P</t>
+  </si>
+  <si>
+    <t>*E</t>
   </si>
 </sst>
 </file>
@@ -610,7 +631,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -640,16 +660,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -661,19 +681,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.4</c:v>
+                  <c:v>0.33</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.3</c:v>
+                  <c:v>0.33</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.28000000000000003</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.35</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -688,11 +708,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="145439744"/>
-        <c:axId val="149172992"/>
+        <c:axId val="134896640"/>
+        <c:axId val="134931200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="145439744"/>
+        <c:axId val="134896640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -704,12 +724,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149172992"/>
+        <c:crossAx val="134931200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="149172992"/>
+        <c:axId val="134931200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -720,7 +740,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145439744"/>
+        <c:crossAx val="134896640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -767,7 +787,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>SimResults!$A$5</c:f>
+              <c:f>SimResults!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -779,7 +799,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>SimResults!$B$5</c:f>
+              <c:f>SimResults!$B$9</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -800,11 +820,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="88070784"/>
-        <c:axId val="88076672"/>
+        <c:axId val="135361664"/>
+        <c:axId val="135363584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="88070784"/>
+        <c:axId val="135361664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -813,7 +833,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88076672"/>
+        <c:crossAx val="135363584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -821,7 +841,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88076672"/>
+        <c:axId val="135363584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -834,7 +854,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88070784"/>
+        <c:crossAx val="135361664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -891,19 +911,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="11" name="Chart 10"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1211,8 +1231,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,7 +1281,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="8">
         <v>40909</v>
@@ -1274,9 +1294,11 @@
         <v>3</v>
       </c>
       <c r="B6" s="7">
-        <v>3000000</v>
-      </c>
-      <c r="C6" s="7"/>
+        <v>100000</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1301,13 +1323,13 @@
         <v>14</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1315,18 +1337,18 @@
         <v>7</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" t="s">
         <v>68</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>69</v>
-      </c>
-      <c r="C11" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1339,30 +1361,40 @@
       <c r="C12" t="s">
         <v>15</v>
       </c>
-      <c r="D12" t="s">
-        <v>67</v>
-      </c>
       <c r="E12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" t="s">
+        <v>166</v>
+      </c>
+      <c r="F13" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
     </row>
   </sheetData>
-  <dataValidations count="9">
+  <dataValidations count="11">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A11">
       <formula1>",,,,,Community Name,,,input,output,Template"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A6">
       <formula1>",,,iterations,,,,,input,output,,Community Name"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A12">
-      <formula1>",,,,,,,,input,output,Start Time,Log File"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A5">
       <formula1>",,,,,,,,input,output,Start Time,Community Name"</formula1>
@@ -1376,8 +1408,17 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A16">
       <formula1>",,,,,Community Name,,,input,output,"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A2">
+      <formula1>",,,,,Community Name,,,input,output,,FlattenApplication"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A9">
+      <formula1>",,,,,Community Name,,,input,output,,output"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A12">
+      <formula1>",,,,,Community Name,,,input,output,,Log File"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A13">
-      <formula1>",,,,,Community Name,,,input,output,"</formula1>
+      <formula1>",,,,,Community Name,,,input,output,,output"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A14">
       <formula1>",,,,,Community Name,,,input,output,"</formula1>
@@ -1601,244 +1642,244 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
         <v>76</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>77</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>78</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>79</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>80</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>81</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>82</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>83</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>84</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>85</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>86</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>87</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>88</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>89</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>90</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>91</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>92</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>93</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>94</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>95</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>96</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>97</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>98</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>99</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>100</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>101</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>102</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>103</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>104</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>105</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>106</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>107</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>108</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>109</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>110</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>111</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>112</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>113</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>114</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>115</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>116</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>117</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>118</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>119</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>120</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>121</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>122</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>123</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>124</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>125</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>126</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>127</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>128</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>129</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>130</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>131</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>132</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>133</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>134</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>135</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>136</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>137</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>138</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>139</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>140</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>141</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BQ1" t="s">
         <v>142</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>143</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>144</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BT1" t="s">
         <v>145</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BU1" t="s">
         <v>146</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BV1" t="s">
         <v>147</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BW1" t="s">
         <v>148</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BX1" t="s">
         <v>149</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="BY1" t="s">
         <v>150</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="BZ1" t="s">
         <v>151</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CA1" t="s">
         <v>152</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CB1" t="s">
         <v>153</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CC1" t="s">
         <v>154</v>
-      </c>
-      <c r="CC1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:81" x14ac:dyDescent="0.25">
@@ -1849,241 +1890,241 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="D2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>0.3</v>
+        <v>0.33</v>
       </c>
       <c r="F2">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>0.28000000000000003</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>0.31</v>
+        <v>0</v>
       </c>
       <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0.33</v>
+      </c>
+      <c r="N2">
         <v>1</v>
       </c>
-      <c r="K2">
-        <v>0.35</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0.4</v>
-      </c>
-      <c r="N2">
-        <v>0.1</v>
-      </c>
       <c r="O2">
-        <v>0.3</v>
+        <v>0.33</v>
       </c>
       <c r="P2">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>0.28000000000000003</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>0.31</v>
+        <v>0</v>
       </c>
       <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0.33</v>
+      </c>
+      <c r="X2">
         <v>1</v>
       </c>
-      <c r="U2">
-        <v>0.35</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0.4</v>
-      </c>
-      <c r="X2">
-        <v>0.1</v>
-      </c>
       <c r="Y2">
-        <v>0.3</v>
+        <v>0.33</v>
       </c>
       <c r="Z2">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="AA2">
-        <v>0.28000000000000003</v>
+        <v>0</v>
       </c>
       <c r="AB2">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="AC2">
-        <v>0.31</v>
+        <v>0</v>
       </c>
       <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0.33</v>
+      </c>
+      <c r="AH2">
         <v>1</v>
       </c>
-      <c r="AE2">
-        <v>0.35</v>
-      </c>
-      <c r="AF2">
-        <v>0</v>
-      </c>
-      <c r="AG2">
-        <v>0.4</v>
-      </c>
-      <c r="AH2">
-        <v>0.1</v>
-      </c>
       <c r="AI2">
-        <v>0.3</v>
+        <v>0.33</v>
       </c>
       <c r="AJ2">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="AK2">
-        <v>0.28000000000000003</v>
+        <v>0</v>
       </c>
       <c r="AL2">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="AM2">
-        <v>0.31</v>
+        <v>0</v>
       </c>
       <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <v>0.33</v>
+      </c>
+      <c r="AR2">
         <v>1</v>
       </c>
-      <c r="AO2">
-        <v>0.35</v>
-      </c>
-      <c r="AP2">
-        <v>0</v>
-      </c>
-      <c r="AQ2">
-        <v>0.4</v>
-      </c>
-      <c r="AR2">
-        <v>0.1</v>
-      </c>
       <c r="AS2">
-        <v>0.3</v>
+        <v>0.33</v>
       </c>
       <c r="AT2">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="AU2">
-        <v>0.28000000000000003</v>
+        <v>0</v>
       </c>
       <c r="AV2">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="AW2">
-        <v>0.31</v>
+        <v>0</v>
       </c>
       <c r="AX2">
+        <v>0</v>
+      </c>
+      <c r="AY2">
+        <v>0</v>
+      </c>
+      <c r="AZ2">
+        <v>0</v>
+      </c>
+      <c r="BA2">
+        <v>0.33</v>
+      </c>
+      <c r="BB2">
         <v>1</v>
       </c>
-      <c r="AY2">
-        <v>0.35</v>
-      </c>
-      <c r="AZ2">
-        <v>0</v>
-      </c>
-      <c r="BA2">
-        <v>0.4</v>
-      </c>
-      <c r="BB2">
-        <v>0.1</v>
-      </c>
       <c r="BC2">
-        <v>0.3</v>
+        <v>0.33</v>
       </c>
       <c r="BD2">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="BE2">
-        <v>0.28000000000000003</v>
+        <v>0</v>
       </c>
       <c r="BF2">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="BG2">
-        <v>0.31</v>
+        <v>0</v>
       </c>
       <c r="BH2">
+        <v>0</v>
+      </c>
+      <c r="BI2">
+        <v>0</v>
+      </c>
+      <c r="BJ2">
+        <v>0</v>
+      </c>
+      <c r="BK2">
+        <v>0.33</v>
+      </c>
+      <c r="BL2">
         <v>1</v>
       </c>
-      <c r="BI2">
-        <v>0.35</v>
-      </c>
-      <c r="BJ2">
-        <v>0</v>
-      </c>
-      <c r="BK2">
-        <v>0.4</v>
-      </c>
-      <c r="BL2">
-        <v>0.1</v>
-      </c>
       <c r="BM2">
-        <v>0.3</v>
+        <v>0.33</v>
       </c>
       <c r="BN2">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="BO2">
-        <v>0.28000000000000003</v>
+        <v>0</v>
       </c>
       <c r="BP2">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="BQ2">
-        <v>0.31</v>
+        <v>0</v>
       </c>
       <c r="BR2">
+        <v>0</v>
+      </c>
+      <c r="BS2">
+        <v>0</v>
+      </c>
+      <c r="BT2">
+        <v>0</v>
+      </c>
+      <c r="BU2">
+        <v>0.33</v>
+      </c>
+      <c r="BV2">
         <v>1</v>
       </c>
-      <c r="BS2">
-        <v>0.35</v>
-      </c>
-      <c r="BT2">
-        <v>0</v>
-      </c>
-      <c r="BU2">
-        <v>0.4</v>
-      </c>
-      <c r="BV2">
-        <v>0.1</v>
-      </c>
       <c r="BW2">
-        <v>0.3</v>
+        <v>0.33</v>
       </c>
       <c r="BX2">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="BY2">
-        <v>0.28000000000000003</v>
+        <v>0</v>
       </c>
       <c r="BZ2">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="CA2">
-        <v>0.31</v>
+        <v>0</v>
       </c>
       <c r="CB2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC2">
-        <v>0.35</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2097,7 +2138,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2324,43 +2365,65 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>158</v>
-      </c>
-      <c r="B5" s="9">
-        <v>1</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>160</v>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B9" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
replaced our original analyser with one modified by PWC; added solar energy totals
</commit_message>
<xml_diff>
--- a/ExcelReader/data/Example.xlsx
+++ b/ExcelReader/data/Example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="390" windowWidth="16005" windowHeight="7545" tabRatio="725"/>
+    <workbookView xWindow="120" yWindow="390" windowWidth="16005" windowHeight="7545" tabRatio="725" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="167">
   <si>
     <t>t</t>
   </si>
@@ -49,9 +49,6 @@
     <t>daly river 1s.csv</t>
   </si>
   <si>
-    <t>week</t>
-  </si>
-  <si>
     <t>..\ExcelReader\bin\Debug\ExcelReader.exe</t>
   </si>
   <si>
@@ -226,9 +223,6 @@
     <t>Template</t>
   </si>
   <si>
-    <t>Analyser.xlsx</t>
-  </si>
-  <si>
     <t>analyse.csv</t>
   </si>
   <si>
@@ -487,43 +481,46 @@
     <t>Gen8FuelCons5L</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>output.csv</t>
+  </si>
+  <si>
+    <t>Solar Load Model  Copyright (C) 2012, 2013  Power Water Corporation.</t>
+  </si>
+  <si>
+    <t>This program comes with ABSOLUTELY NO WARRANTY;</t>
+  </si>
+  <si>
+    <t>This is free software, and you are welcome to redistribute it</t>
+  </si>
+  <si>
+    <t>under certain conditions; see the file COPYING for details.</t>
+  </si>
+  <si>
+    <t>*P</t>
+  </si>
+  <si>
+    <t>*E</t>
+  </si>
+  <si>
+    <t>Analyser Layout Redifined V.4.xls</t>
+  </si>
+  <si>
+    <t>Run started on 10/01/2013 6:44:27 PM</t>
+  </si>
+  <si>
     <t>Init...</t>
   </si>
   <si>
+    <t>Run 345600 iterations...</t>
+  </si>
+  <si>
     <t>Percent Complete</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>output.csv</t>
-  </si>
-  <si>
-    <t>Run 100000 iterations...</t>
-  </si>
-  <si>
-    <t>Run started on 10/01/2013 5:21:08 PM</t>
-  </si>
-  <si>
-    <t>Solar Load Model  Copyright (C) 2012, 2013  Power Water Corporation.</t>
-  </si>
-  <si>
-    <t>This program comes with ABSOLUTELY NO WARRANTY;</t>
-  </si>
-  <si>
-    <t>This is free software, and you are welcome to redistribute it</t>
-  </si>
-  <si>
-    <t>under certain conditions; see the file COPYING for details.</t>
-  </si>
-  <si>
-    <t>inner loop took 11.6191618s</t>
-  </si>
-  <si>
-    <t>*P</t>
-  </si>
-  <si>
-    <t>*E</t>
+    <t>inner loop took 19.0869085s</t>
   </si>
 </sst>
 </file>
@@ -708,11 +705,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="134896640"/>
-        <c:axId val="134931200"/>
+        <c:axId val="148347904"/>
+        <c:axId val="147989248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="134896640"/>
+        <c:axId val="148347904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -724,12 +721,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134931200"/>
+        <c:crossAx val="147989248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="134931200"/>
+        <c:axId val="147989248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -740,7 +737,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134896640"/>
+        <c:crossAx val="148347904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -820,11 +817,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="135361664"/>
-        <c:axId val="135363584"/>
+        <c:axId val="5470464"/>
+        <c:axId val="5472256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="135361664"/>
+        <c:axId val="5470464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -833,7 +830,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135363584"/>
+        <c:crossAx val="5472256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -841,7 +838,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="135363584"/>
+        <c:axId val="5472256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -854,7 +851,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135361664"/>
+        <c:crossAx val="5470464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -911,19 +908,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="11" name="Chart 10"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1231,8 +1228,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1259,7 +1256,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1267,7 +1264,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1275,13 +1272,13 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5" s="8">
         <v>40909</v>
@@ -1294,10 +1291,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="7">
-        <v>100000</v>
+        <v>345600</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1315,21 +1312,24 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
+        <v>67</v>
+      </c>
+      <c r="C9">
+        <v>86400</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>68</v>
+      </c>
+      <c r="E9" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1337,52 +1337,52 @@
         <v>7</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C11" t="s">
         <v>67</v>
-      </c>
-      <c r="B11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" t="s">
         <v>65</v>
       </c>
-      <c r="B12" t="s">
-        <v>66</v>
-      </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E13" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="F13" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1452,85 +1452,85 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="M1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="T1" s="6" t="s">
-        <v>52</v>
-      </c>
       <c r="U1" t="s">
+        <v>56</v>
+      </c>
+      <c r="V1" t="s">
         <v>57</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>58</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>59</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>60</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>61</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>62</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>63</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -1642,244 +1642,244 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" t="s">
         <v>75</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>76</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>77</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>78</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>79</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>80</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>81</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>82</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>83</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>84</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>85</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>86</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>87</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>88</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>89</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>90</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>91</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>92</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>93</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>94</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>95</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>96</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>97</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>98</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>99</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>100</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>101</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>102</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>103</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>104</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>105</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>106</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>107</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>108</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>109</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>110</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>111</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>112</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AP1" t="s">
         <v>113</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AQ1" t="s">
         <v>114</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AR1" t="s">
         <v>115</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AS1" t="s">
         <v>116</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AT1" t="s">
         <v>117</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AU1" t="s">
         <v>118</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AV1" t="s">
         <v>119</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AW1" t="s">
         <v>120</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AX1" t="s">
         <v>121</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AY1" t="s">
         <v>122</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AZ1" t="s">
         <v>123</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BA1" t="s">
         <v>124</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BB1" t="s">
         <v>125</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BC1" t="s">
         <v>126</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BD1" t="s">
         <v>127</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BE1" t="s">
         <v>128</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BF1" t="s">
         <v>129</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BG1" t="s">
         <v>130</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BH1" t="s">
         <v>131</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BI1" t="s">
         <v>132</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BJ1" t="s">
         <v>133</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BK1" t="s">
         <v>134</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BL1" t="s">
         <v>135</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BM1" t="s">
         <v>136</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BN1" t="s">
         <v>137</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BO1" t="s">
         <v>138</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BP1" t="s">
         <v>139</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BQ1" t="s">
         <v>140</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BR1" t="s">
         <v>141</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BS1" t="s">
         <v>142</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BT1" t="s">
         <v>143</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BU1" t="s">
         <v>144</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BV1" t="s">
         <v>145</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BW1" t="s">
         <v>146</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BX1" t="s">
         <v>147</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BY1" t="s">
         <v>148</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="BZ1" t="s">
         <v>149</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="CA1" t="s">
         <v>150</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CB1" t="s">
         <v>151</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CC1" t="s">
         <v>152</v>
-      </c>
-      <c r="CB1" t="s">
-        <v>153</v>
-      </c>
-      <c r="CC1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:81" x14ac:dyDescent="0.25">
@@ -2150,10 +2150,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2190,61 +2190,61 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>32</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>33</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>34</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>35</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>36</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>37</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>38</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>39</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>41</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>42</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>43</v>
-      </c>
-      <c r="T1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -2340,10 +2340,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
         <v>54</v>
-      </c>
-      <c r="C1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2367,55 +2367,55 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="B9" s="9">
         <v>1</v>
@@ -2423,7 +2423,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated with new example files.
</commit_message>
<xml_diff>
--- a/ExcelReader/data/Example.xlsx
+++ b/ExcelReader/data/Example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="390" windowWidth="16005" windowHeight="7545" tabRatio="725" activeTab="6"/>
+    <workbookView xWindow="120" yWindow="390" windowWidth="16005" windowHeight="7545" tabRatio="725"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="173">
   <si>
     <t>t</t>
   </si>
@@ -46,9 +46,6 @@
     <t>RunSimulator</t>
   </si>
   <si>
-    <t>daly river 1s.csv</t>
-  </si>
-  <si>
     <t>..\ExcelReader\bin\Debug\ExcelReader.exe</t>
   </si>
   <si>
@@ -178,9 +175,6 @@
     <t>Gen8MinRunTPa</t>
   </si>
   <si>
-    <t>daly river Pv 1s.csv</t>
-  </si>
-  <si>
     <t>PvSetMaxDownP</t>
   </si>
   <si>
@@ -220,307 +214,331 @@
     <t>log_entries.txt</t>
   </si>
   <si>
+    <t>analyse.csv</t>
+  </si>
+  <si>
+    <t>*Cnt</t>
+  </si>
+  <si>
+    <t>This sheet is automatically filled.  Any edits will be lost each time you run the Simulator</t>
+  </si>
+  <si>
+    <t>GenConfig*</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Start Time</t>
+  </si>
+  <si>
+    <t>Gen1FuelCons1P</t>
+  </si>
+  <si>
+    <t>Gen1FuelCons1L</t>
+  </si>
+  <si>
+    <t>Gen1FuelCons2P</t>
+  </si>
+  <si>
+    <t>Gen1FuelCons2L</t>
+  </si>
+  <si>
+    <t>Gen1FuelCons3P</t>
+  </si>
+  <si>
+    <t>Gen1FuelCons3L</t>
+  </si>
+  <si>
+    <t>Gen1FuelCons4P</t>
+  </si>
+  <si>
+    <t>Gen1FuelCons4L</t>
+  </si>
+  <si>
+    <t>Gen1FuelCons5P</t>
+  </si>
+  <si>
+    <t>Gen1FuelCons5L</t>
+  </si>
+  <si>
+    <t>Gen2FuelCons1P</t>
+  </si>
+  <si>
+    <t>Gen2FuelCons1L</t>
+  </si>
+  <si>
+    <t>Gen2FuelCons2P</t>
+  </si>
+  <si>
+    <t>Gen2FuelCons2L</t>
+  </si>
+  <si>
+    <t>Gen2FuelCons3P</t>
+  </si>
+  <si>
+    <t>Gen2FuelCons3L</t>
+  </si>
+  <si>
+    <t>Gen2FuelCons4P</t>
+  </si>
+  <si>
+    <t>Gen2FuelCons4L</t>
+  </si>
+  <si>
+    <t>Gen2FuelCons5P</t>
+  </si>
+  <si>
+    <t>Gen2FuelCons5L</t>
+  </si>
+  <si>
+    <t>Gen3FuelCons1P</t>
+  </si>
+  <si>
+    <t>Gen3FuelCons1L</t>
+  </si>
+  <si>
+    <t>Gen3FuelCons2P</t>
+  </si>
+  <si>
+    <t>Gen3FuelCons2L</t>
+  </si>
+  <si>
+    <t>Gen3FuelCons3P</t>
+  </si>
+  <si>
+    <t>Gen3FuelCons3L</t>
+  </si>
+  <si>
+    <t>Gen3FuelCons4P</t>
+  </si>
+  <si>
+    <t>Gen3FuelCons4L</t>
+  </si>
+  <si>
+    <t>Gen3FuelCons5P</t>
+  </si>
+  <si>
+    <t>Gen3FuelCons5L</t>
+  </si>
+  <si>
+    <t>Gen4FuelCons1P</t>
+  </si>
+  <si>
+    <t>Gen4FuelCons1L</t>
+  </si>
+  <si>
+    <t>Gen4FuelCons2P</t>
+  </si>
+  <si>
+    <t>Gen4FuelCons2L</t>
+  </si>
+  <si>
+    <t>Gen4FuelCons3P</t>
+  </si>
+  <si>
+    <t>Gen4FuelCons3L</t>
+  </si>
+  <si>
+    <t>Gen4FuelCons4P</t>
+  </si>
+  <si>
+    <t>Gen4FuelCons4L</t>
+  </si>
+  <si>
+    <t>Gen4FuelCons5P</t>
+  </si>
+  <si>
+    <t>Gen4FuelCons5L</t>
+  </si>
+  <si>
+    <t>Gen5FuelCons1P</t>
+  </si>
+  <si>
+    <t>Gen5FuelCons1L</t>
+  </si>
+  <si>
+    <t>Gen5FuelCons2P</t>
+  </si>
+  <si>
+    <t>Gen5FuelCons2L</t>
+  </si>
+  <si>
+    <t>Gen5FuelCons3P</t>
+  </si>
+  <si>
+    <t>Gen5FuelCons3L</t>
+  </si>
+  <si>
+    <t>Gen5FuelCons4P</t>
+  </si>
+  <si>
+    <t>Gen5FuelCons4L</t>
+  </si>
+  <si>
+    <t>Gen5FuelCons5P</t>
+  </si>
+  <si>
+    <t>Gen5FuelCons5L</t>
+  </si>
+  <si>
+    <t>Gen6FuelCons1P</t>
+  </si>
+  <si>
+    <t>Gen6FuelCons1L</t>
+  </si>
+  <si>
+    <t>Gen6FuelCons2P</t>
+  </si>
+  <si>
+    <t>Gen6FuelCons2L</t>
+  </si>
+  <si>
+    <t>Gen6FuelCons3P</t>
+  </si>
+  <si>
+    <t>Gen6FuelCons3L</t>
+  </si>
+  <si>
+    <t>Gen6FuelCons4P</t>
+  </si>
+  <si>
+    <t>Gen6FuelCons4L</t>
+  </si>
+  <si>
+    <t>Gen6FuelCons5P</t>
+  </si>
+  <si>
+    <t>Gen6FuelCons5L</t>
+  </si>
+  <si>
+    <t>Gen7FuelCons1P</t>
+  </si>
+  <si>
+    <t>Gen7FuelCons1L</t>
+  </si>
+  <si>
+    <t>Gen7FuelCons2P</t>
+  </si>
+  <si>
+    <t>Gen7FuelCons2L</t>
+  </si>
+  <si>
+    <t>Gen7FuelCons3P</t>
+  </si>
+  <si>
+    <t>Gen7FuelCons3L</t>
+  </si>
+  <si>
+    <t>Gen7FuelCons4P</t>
+  </si>
+  <si>
+    <t>Gen7FuelCons4L</t>
+  </si>
+  <si>
+    <t>Gen7FuelCons5P</t>
+  </si>
+  <si>
+    <t>Gen7FuelCons5L</t>
+  </si>
+  <si>
+    <t>Gen8FuelCons1P</t>
+  </si>
+  <si>
+    <t>Gen8FuelCons1L</t>
+  </si>
+  <si>
+    <t>Gen8FuelCons2P</t>
+  </si>
+  <si>
+    <t>Gen8FuelCons2L</t>
+  </si>
+  <si>
+    <t>Gen8FuelCons3P</t>
+  </si>
+  <si>
+    <t>Gen8FuelCons3L</t>
+  </si>
+  <si>
+    <t>Gen8FuelCons4P</t>
+  </si>
+  <si>
+    <t>Gen8FuelCons4L</t>
+  </si>
+  <si>
+    <t>Gen8FuelCons5P</t>
+  </si>
+  <si>
+    <t>Gen8FuelCons5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Solar Load Model  Copyright (C) 2012, 2013  Power Water Corporation.</t>
+  </si>
+  <si>
+    <t>This program comes with ABSOLUTELY NO WARRANTY;</t>
+  </si>
+  <si>
+    <t>This is free software, and you are welcome to redistribute it</t>
+  </si>
+  <si>
+    <t>under certain conditions; see the file COPYING for details.</t>
+  </si>
+  <si>
+    <t>*E</t>
+  </si>
+  <si>
+    <t>Init...</t>
+  </si>
+  <si>
+    <t>Percent Complete</t>
+  </si>
+  <si>
+    <t>Watch</t>
+  </si>
+  <si>
+    <t>watchfile.txt</t>
+  </si>
+  <si>
+    <t>version 2013/01/23-18819</t>
+  </si>
+  <si>
+    <t>Run 172800 iterations...</t>
+  </si>
+  <si>
+    <t>load.csv</t>
+  </si>
+  <si>
+    <t>renewables.csv</t>
+  </si>
+  <si>
     <t>Template</t>
   </si>
   <si>
-    <t>analyse.csv</t>
-  </si>
-  <si>
-    <t>*Cnt</t>
-  </si>
-  <si>
-    <t>This sheet is automatically filled.  Any edits will be lost each time you run the Simulator</t>
-  </si>
-  <si>
-    <t>GenConfig*</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Start Time</t>
-  </si>
-  <si>
-    <t>Gen1FuelCons1P</t>
-  </si>
-  <si>
-    <t>Gen1FuelCons1L</t>
-  </si>
-  <si>
-    <t>Gen1FuelCons2P</t>
-  </si>
-  <si>
-    <t>Gen1FuelCons2L</t>
-  </si>
-  <si>
-    <t>Gen1FuelCons3P</t>
-  </si>
-  <si>
-    <t>Gen1FuelCons3L</t>
-  </si>
-  <si>
-    <t>Gen1FuelCons4P</t>
-  </si>
-  <si>
-    <t>Gen1FuelCons4L</t>
-  </si>
-  <si>
-    <t>Gen1FuelCons5P</t>
-  </si>
-  <si>
-    <t>Gen1FuelCons5L</t>
-  </si>
-  <si>
-    <t>Gen2FuelCons1P</t>
-  </si>
-  <si>
-    <t>Gen2FuelCons1L</t>
-  </si>
-  <si>
-    <t>Gen2FuelCons2P</t>
-  </si>
-  <si>
-    <t>Gen2FuelCons2L</t>
-  </si>
-  <si>
-    <t>Gen2FuelCons3P</t>
-  </si>
-  <si>
-    <t>Gen2FuelCons3L</t>
-  </si>
-  <si>
-    <t>Gen2FuelCons4P</t>
-  </si>
-  <si>
-    <t>Gen2FuelCons4L</t>
-  </si>
-  <si>
-    <t>Gen2FuelCons5P</t>
-  </si>
-  <si>
-    <t>Gen2FuelCons5L</t>
-  </si>
-  <si>
-    <t>Gen3FuelCons1P</t>
-  </si>
-  <si>
-    <t>Gen3FuelCons1L</t>
-  </si>
-  <si>
-    <t>Gen3FuelCons2P</t>
-  </si>
-  <si>
-    <t>Gen3FuelCons2L</t>
-  </si>
-  <si>
-    <t>Gen3FuelCons3P</t>
-  </si>
-  <si>
-    <t>Gen3FuelCons3L</t>
-  </si>
-  <si>
-    <t>Gen3FuelCons4P</t>
-  </si>
-  <si>
-    <t>Gen3FuelCons4L</t>
-  </si>
-  <si>
-    <t>Gen3FuelCons5P</t>
-  </si>
-  <si>
-    <t>Gen3FuelCons5L</t>
-  </si>
-  <si>
-    <t>Gen4FuelCons1P</t>
-  </si>
-  <si>
-    <t>Gen4FuelCons1L</t>
-  </si>
-  <si>
-    <t>Gen4FuelCons2P</t>
-  </si>
-  <si>
-    <t>Gen4FuelCons2L</t>
-  </si>
-  <si>
-    <t>Gen4FuelCons3P</t>
-  </si>
-  <si>
-    <t>Gen4FuelCons3L</t>
-  </si>
-  <si>
-    <t>Gen4FuelCons4P</t>
-  </si>
-  <si>
-    <t>Gen4FuelCons4L</t>
-  </si>
-  <si>
-    <t>Gen4FuelCons5P</t>
-  </si>
-  <si>
-    <t>Gen4FuelCons5L</t>
-  </si>
-  <si>
-    <t>Gen5FuelCons1P</t>
-  </si>
-  <si>
-    <t>Gen5FuelCons1L</t>
-  </si>
-  <si>
-    <t>Gen5FuelCons2P</t>
-  </si>
-  <si>
-    <t>Gen5FuelCons2L</t>
-  </si>
-  <si>
-    <t>Gen5FuelCons3P</t>
-  </si>
-  <si>
-    <t>Gen5FuelCons3L</t>
-  </si>
-  <si>
-    <t>Gen5FuelCons4P</t>
-  </si>
-  <si>
-    <t>Gen5FuelCons4L</t>
-  </si>
-  <si>
-    <t>Gen5FuelCons5P</t>
-  </si>
-  <si>
-    <t>Gen5FuelCons5L</t>
-  </si>
-  <si>
-    <t>Gen6FuelCons1P</t>
-  </si>
-  <si>
-    <t>Gen6FuelCons1L</t>
-  </si>
-  <si>
-    <t>Gen6FuelCons2P</t>
-  </si>
-  <si>
-    <t>Gen6FuelCons2L</t>
-  </si>
-  <si>
-    <t>Gen6FuelCons3P</t>
-  </si>
-  <si>
-    <t>Gen6FuelCons3L</t>
-  </si>
-  <si>
-    <t>Gen6FuelCons4P</t>
-  </si>
-  <si>
-    <t>Gen6FuelCons4L</t>
-  </si>
-  <si>
-    <t>Gen6FuelCons5P</t>
-  </si>
-  <si>
-    <t>Gen6FuelCons5L</t>
-  </si>
-  <si>
-    <t>Gen7FuelCons1P</t>
-  </si>
-  <si>
-    <t>Gen7FuelCons1L</t>
-  </si>
-  <si>
-    <t>Gen7FuelCons2P</t>
-  </si>
-  <si>
-    <t>Gen7FuelCons2L</t>
-  </si>
-  <si>
-    <t>Gen7FuelCons3P</t>
-  </si>
-  <si>
-    <t>Gen7FuelCons3L</t>
-  </si>
-  <si>
-    <t>Gen7FuelCons4P</t>
-  </si>
-  <si>
-    <t>Gen7FuelCons4L</t>
-  </si>
-  <si>
-    <t>Gen7FuelCons5P</t>
-  </si>
-  <si>
-    <t>Gen7FuelCons5L</t>
-  </si>
-  <si>
-    <t>Gen8FuelCons1P</t>
-  </si>
-  <si>
-    <t>Gen8FuelCons1L</t>
-  </si>
-  <si>
-    <t>Gen8FuelCons2P</t>
-  </si>
-  <si>
-    <t>Gen8FuelCons2L</t>
-  </si>
-  <si>
-    <t>Gen8FuelCons3P</t>
-  </si>
-  <si>
-    <t>Gen8FuelCons3L</t>
-  </si>
-  <si>
-    <t>Gen8FuelCons4P</t>
-  </si>
-  <si>
-    <t>Gen8FuelCons4L</t>
-  </si>
-  <si>
-    <t>Gen8FuelCons5P</t>
-  </si>
-  <si>
-    <t>Gen8FuelCons5L</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>output.csv</t>
-  </si>
-  <si>
-    <t>Solar Load Model  Copyright (C) 2012, 2013  Power Water Corporation.</t>
-  </si>
-  <si>
-    <t>This program comes with ABSOLUTELY NO WARRANTY;</t>
-  </si>
-  <si>
-    <t>This is free software, and you are welcome to redistribute it</t>
-  </si>
-  <si>
-    <t>under certain conditions; see the file COPYING for details.</t>
-  </si>
-  <si>
-    <t>*P</t>
-  </si>
-  <si>
-    <t>*E</t>
-  </si>
-  <si>
-    <t>Analyser Layout Redifined V.4.xls</t>
-  </si>
-  <si>
-    <t>Run started on 10/01/2013 6:44:27 PM</t>
-  </si>
-  <si>
-    <t>Init...</t>
-  </si>
-  <si>
-    <t>Run 345600 iterations...</t>
-  </si>
-  <si>
-    <t>Percent Complete</t>
-  </si>
-  <si>
-    <t>inner loop took 19.0869085s</t>
+    <t>NPV Analyser.xls</t>
+  </si>
+  <si>
+    <t>*MaxP</t>
+  </si>
+  <si>
+    <t>*SetP</t>
+  </si>
+  <si>
+    <t>*Cfg</t>
+  </si>
+  <si>
+    <t>*Pa</t>
+  </si>
+  <si>
+    <t>Gen[1-2]StartCnt</t>
+  </si>
+  <si>
+    <t>Run started on 23/01/2013 2:47:03 PM</t>
+  </si>
+  <si>
+    <t>inner loop took 0.8810504s</t>
   </si>
 </sst>
 </file>
@@ -628,6 +646,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -705,11 +724,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="148347904"/>
-        <c:axId val="147989248"/>
+        <c:axId val="73736192"/>
+        <c:axId val="73756032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="148347904"/>
+        <c:axId val="73736192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -721,12 +740,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147989248"/>
+        <c:crossAx val="73756032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="147989248"/>
+        <c:axId val="73756032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -737,7 +756,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148347904"/>
+        <c:crossAx val="73736192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -784,7 +803,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>SimResults!$A$9</c:f>
+              <c:f>SimResults!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -796,7 +815,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>SimResults!$B$9</c:f>
+              <c:f>SimResults!$B$10</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -817,11 +836,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="5470464"/>
-        <c:axId val="5472256"/>
+        <c:axId val="100074240"/>
+        <c:axId val="100075776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="5470464"/>
+        <c:axId val="100074240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -830,7 +849,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="5472256"/>
+        <c:crossAx val="100075776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -838,7 +857,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="5472256"/>
+        <c:axId val="100075776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -851,7 +870,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="5470464"/>
+        <c:crossAx val="100074240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -909,18 +928,18 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1226,11 +1245,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1245,40 +1262,40 @@
     <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="7"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B5" s="8">
         <v>40909</v>
@@ -1286,113 +1303,110 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="7">
-        <v>345600</v>
+        <v>172800</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>8</v>
+      <c r="B7" s="7" t="s">
+        <v>162</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C9">
-        <v>86400</v>
+        <v>604800</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E9" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>164</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" t="s">
+        <v>166</v>
+      </c>
+      <c r="D12" t="s">
+        <v>167</v>
+      </c>
+      <c r="E12" t="s">
+        <v>168</v>
+      </c>
+      <c r="F12" t="s">
+        <v>169</v>
+      </c>
+      <c r="G12" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>158</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" t="s">
         <v>159</v>
       </c>
-      <c r="F13" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
     </row>
   </sheetData>
-  <dataValidations count="11">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A11">
-      <formula1>",,,,,Community Name,,,input,output,Template"</formula1>
-    </dataValidation>
+  <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A6">
       <formula1>",,,iterations,,,,,input,output,,Community Name"</formula1>
     </dataValidation>
@@ -1402,30 +1416,27 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B10">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A15">
-      <formula1>",,,,,Community Name,,,input,output,"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A16">
-      <formula1>",,,,,Community Name,,,input,output,"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A9">
+      <formula1>",,,,,Community Name,,,input,output,,output"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A2">
       <formula1>",,,,,Community Name,,,input,output,,FlattenApplication"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A9">
-      <formula1>",,,,,Community Name,,,input,output,,output"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A12">
-      <formula1>",,,,,Community Name,,,input,output,,Log File"</formula1>
+      <formula1>",,,,,Community Name,Template,,input,output,,,Log File"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A13">
-      <formula1>",,,,,Community Name,,,input,output,,output"</formula1>
+      <formula1>",,,,,Community Name,Template,,input,output,,,Watch"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A14">
-      <formula1>",,,,,Community Name,,,input,output,"</formula1>
+      <formula1>",,,,,Community Name,Template,,input,output,,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A11">
+      <formula1>",,,,,Community Name,Template,,input,output,,"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1452,85 +1463,85 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="M1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="T1" s="6" t="s">
-        <v>51</v>
-      </c>
       <c r="U1" t="s">
+        <v>54</v>
+      </c>
+      <c r="V1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W1" t="s">
         <v>56</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>57</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>58</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>59</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>60</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>61</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -1629,7 +1640,9 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:CC2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1642,244 +1655,244 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" t="s">
         <v>73</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>74</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>75</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>76</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>77</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>78</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>79</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>83</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>84</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>85</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>86</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>87</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>88</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>89</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>90</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>91</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>92</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>93</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>94</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>95</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>96</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
         <v>97</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>98</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AE1" t="s">
         <v>99</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AF1" t="s">
         <v>100</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AG1" t="s">
         <v>101</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AH1" t="s">
         <v>102</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AI1" t="s">
         <v>103</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AJ1" t="s">
         <v>104</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>105</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AL1" t="s">
         <v>106</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AM1" t="s">
         <v>107</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AN1" t="s">
         <v>108</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AO1" t="s">
         <v>109</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AP1" t="s">
         <v>110</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AQ1" t="s">
         <v>111</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AR1" t="s">
         <v>112</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AS1" t="s">
         <v>113</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AT1" t="s">
         <v>114</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AU1" t="s">
         <v>115</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AV1" t="s">
         <v>116</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AW1" t="s">
         <v>117</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AX1" t="s">
         <v>118</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AY1" t="s">
         <v>119</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AZ1" t="s">
         <v>120</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BA1" t="s">
         <v>121</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BB1" t="s">
         <v>122</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BC1" t="s">
         <v>123</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BD1" t="s">
         <v>124</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BE1" t="s">
         <v>125</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BF1" t="s">
         <v>126</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BG1" t="s">
         <v>127</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BH1" t="s">
         <v>128</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BI1" t="s">
         <v>129</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BJ1" t="s">
         <v>130</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BK1" t="s">
         <v>131</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BL1" t="s">
         <v>132</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BM1" t="s">
         <v>133</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BN1" t="s">
         <v>134</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BO1" t="s">
         <v>135</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BP1" t="s">
         <v>136</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BQ1" t="s">
         <v>137</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BR1" t="s">
         <v>138</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BS1" t="s">
         <v>139</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BT1" t="s">
         <v>140</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BU1" t="s">
         <v>141</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BV1" t="s">
         <v>142</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BW1" t="s">
         <v>143</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BX1" t="s">
         <v>144</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BY1" t="s">
         <v>145</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BZ1" t="s">
         <v>146</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="CA1" t="s">
         <v>147</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="CB1" t="s">
         <v>148</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CC1" t="s">
         <v>149</v>
-      </c>
-      <c r="CA1" t="s">
-        <v>150</v>
-      </c>
-      <c r="CB1" t="s">
-        <v>151</v>
-      </c>
-      <c r="CC1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:81" x14ac:dyDescent="0.25">
@@ -2150,10 +2163,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2190,61 +2203,61 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>32</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>33</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>34</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>35</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>36</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>37</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>38</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>39</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>40</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>41</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>42</v>
-      </c>
-      <c r="T1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -2340,10 +2353,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2365,65 +2378,70 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>165</v>
-      </c>
-      <c r="B9" s="9">
-        <v>1</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>166</v>
+        <v>157</v>
+      </c>
+      <c r="B10" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added GenAvailSet to represent user's available generator parameter, so GenAvailCfg can become the system available generator parameter. Fixed service outage bug.  Also added Gen#ServiceOutT - the time it takes to service a generator.
</commit_message>
<xml_diff>
--- a/ExcelReader/data/Example.xlsx
+++ b/ExcelReader/data/Example.xlsx
@@ -55,9 +55,6 @@
     <t>..\..\SolarLoadModel\Data</t>
   </si>
   <si>
-    <t>GenAvailCfg</t>
-  </si>
-  <si>
     <t>output</t>
   </si>
   <si>
@@ -539,6 +536,9 @@
   </si>
   <si>
     <t>inner loop took 2.3851365s</t>
+  </si>
+  <si>
+    <t>GenAvailSet</t>
   </si>
 </sst>
 </file>
@@ -723,11 +723,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="73824896"/>
-        <c:axId val="73836032"/>
+        <c:axId val="94780032"/>
+        <c:axId val="102553088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73824896"/>
+        <c:axId val="94780032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -739,12 +739,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73836032"/>
+        <c:crossAx val="102553088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73836032"/>
+        <c:axId val="102553088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -755,7 +755,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73824896"/>
+        <c:crossAx val="94780032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -787,7 +787,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -835,11 +834,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="117375360"/>
-        <c:axId val="117377280"/>
+        <c:axId val="107975808"/>
+        <c:axId val="107977728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="117375360"/>
+        <c:axId val="107975808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -848,7 +847,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117377280"/>
+        <c:crossAx val="107977728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -856,7 +855,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117377280"/>
+        <c:axId val="107977728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -869,7 +868,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117375360"/>
+        <c:crossAx val="107975808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1294,7 +1293,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5" s="8">
         <v>41196.600694444445</v>
@@ -1310,7 +1309,7 @@
         <v>172800</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1318,7 +1317,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -1328,24 +1327,24 @@
         <v>6</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9">
         <v>604800</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1353,52 +1352,52 @@
         <v>7</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>163</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>165</v>
-      </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" t="s">
         <v>62</v>
       </c>
-      <c r="B12" t="s">
-        <v>63</v>
-      </c>
       <c r="C12" t="s">
+        <v>165</v>
+      </c>
+      <c r="D12" t="s">
         <v>166</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>167</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>168</v>
       </c>
-      <c r="F12" t="s">
-        <v>169</v>
-      </c>
       <c r="G12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>157</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>159</v>
-      </c>
       <c r="C13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1447,7 +1446,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1465,85 +1466,85 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>172</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="M1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="T1" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="U1" t="s">
+        <v>53</v>
+      </c>
+      <c r="V1" t="s">
         <v>54</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>55</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>56</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>57</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>58</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>59</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>60</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -1657,244 +1658,244 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" t="s">
         <v>70</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>71</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>72</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>73</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>74</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>75</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>76</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>77</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>78</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>79</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>80</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>81</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>82</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>83</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>84</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>85</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>86</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>87</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>88</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>89</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>90</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>91</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>92</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>93</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>94</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>95</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>96</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>97</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>98</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>99</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>100</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>101</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>102</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>103</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>104</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>105</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>106</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>107</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>108</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>109</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>110</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>111</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>112</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>113</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>114</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>115</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>116</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>117</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>118</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>119</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>120</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>121</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>122</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>123</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>124</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>125</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>126</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>127</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>128</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>129</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>130</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>131</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>132</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>133</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>134</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>135</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BQ1" t="s">
         <v>136</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>137</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>138</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BT1" t="s">
         <v>139</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BU1" t="s">
         <v>140</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BV1" t="s">
         <v>141</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BW1" t="s">
         <v>142</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BX1" t="s">
         <v>143</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="BY1" t="s">
         <v>144</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="BZ1" t="s">
         <v>145</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CA1" t="s">
         <v>146</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CB1" t="s">
         <v>147</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CC1" t="s">
         <v>148</v>
-      </c>
-      <c r="CC1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:81" x14ac:dyDescent="0.25">
@@ -2165,10 +2166,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2205,61 +2206,61 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>27</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>29</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>30</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>31</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>32</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>33</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>34</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>35</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>36</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>37</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>38</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>39</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>40</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>41</v>
-      </c>
-      <c r="T1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -2355,10 +2356,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
         <v>51</v>
-      </c>
-      <c r="C1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2390,52 +2391,52 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B10" s="9">
         <v>1</v>
@@ -2443,7 +2444,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more work on algorithm and generator validation modes; fixed minor text output and spreadsheet formatting things; fixed GenAvailSet bug; fixed fuel curve 0,0 point issue; updated user manual
</commit_message>
<xml_diff>
--- a/ExcelReader/data/Example.xlsx
+++ b/ExcelReader/data/Example.xlsx
@@ -499,9 +499,6 @@
     <t>watchfile.txt</t>
   </si>
   <si>
-    <t>version 2013/01/23-18819</t>
-  </si>
-  <si>
     <t>Run 172800 iterations...</t>
   </si>
   <si>
@@ -532,13 +529,16 @@
     <t>Gen[1-4]StartCnt</t>
   </si>
   <si>
-    <t>Run started on 23/01/2013 2:56:15 PM</t>
-  </si>
-  <si>
-    <t>inner loop took 2.3851365s</t>
-  </si>
-  <si>
     <t>GenAvailSet</t>
+  </si>
+  <si>
+    <t>Run started on 25/02/2013 8:21:13 AM</t>
+  </si>
+  <si>
+    <t>version 2013/02/22-20662</t>
+  </si>
+  <si>
+    <t>inner loop took 1.70017s</t>
   </si>
 </sst>
 </file>
@@ -723,11 +723,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="94780032"/>
-        <c:axId val="102553088"/>
+        <c:axId val="186153984"/>
+        <c:axId val="185996032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94780032"/>
+        <c:axId val="186153984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -739,12 +739,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102553088"/>
+        <c:crossAx val="185996032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="102553088"/>
+        <c:axId val="185996032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -755,7 +755,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94780032"/>
+        <c:crossAx val="186153984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -787,6 +787,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -834,11 +835,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="107975808"/>
-        <c:axId val="107977728"/>
+        <c:axId val="61489152"/>
+        <c:axId val="61490688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="107975808"/>
+        <c:axId val="61489152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -847,7 +848,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107977728"/>
+        <c:crossAx val="61490688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -855,7 +856,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107977728"/>
+        <c:axId val="61490688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -868,7 +869,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107975808"/>
+        <c:crossAx val="61489152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -937,7 +938,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1243,9 +1244,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1317,7 +1320,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -1327,7 +1330,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1357,10 +1360,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>163</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>164</v>
       </c>
       <c r="C11" t="s">
         <v>63</v>
@@ -1374,16 +1377,16 @@
         <v>62</v>
       </c>
       <c r="C12" t="s">
+        <v>164</v>
+      </c>
+      <c r="D12" t="s">
         <v>165</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>166</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>167</v>
-      </c>
-      <c r="F12" t="s">
-        <v>168</v>
       </c>
       <c r="G12" t="s">
         <v>66</v>
@@ -1397,14 +1400,11 @@
         <v>158</v>
       </c>
       <c r="C13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="7"/>
     </row>
   </sheetData>
   <dataValidations count="9">
@@ -1429,11 +1429,11 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A13">
       <formula1>",,,,,Community Name,Template,,input,output,,,Watch"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A11">
       <formula1>",,,,,Community Name,Template,,input,output,,"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A11">
-      <formula1>",,,,,Community Name,Template,,input,output,,"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A14">
+      <formula1>",,,,,Community Name,,,input,output,,,Parameter"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1490,7 +1490,7 @@
         <v>19</v>
       </c>
       <c r="J1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>20</v>
@@ -2421,7 +2421,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2431,7 +2431,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2444,7 +2444,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>